<commit_message>
modify bubble fault seed`
</commit_message>
<xml_diff>
--- a/bubble_fault_seeded.xlsx
+++ b/bubble_fault_seeded.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <r>
       <t>if (array[d] &gt; array</t>
@@ -324,12 +324,6 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -339,6 +333,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="31">
@@ -701,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:F27"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -718,433 +718,220 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1"/>
-      <c r="B4" s="3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
         <v>9</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30">
-      <c r="A5" s="1"/>
-      <c r="B5" s="3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="D5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
         <v>0</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="1"/>
-      <c r="B6" s="3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1">
         <v>11</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="1"/>
-      <c r="B7" s="3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="1">
         <v>5</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
         <v>12</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="3">
-        <v>1</v>
-      </c>
-      <c r="F7" s="3">
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="1"/>
-      <c r="B8" s="3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="1">
         <v>6</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="1">
         <v>23</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="3">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3">
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="1"/>
-      <c r="B9" s="3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="1">
         <v>7</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="1">
         <v>25</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="3">
-        <v>1</v>
-      </c>
-      <c r="F9" s="3">
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="1"/>
-      <c r="B10" s="3">
+      <c r="A10" s="5"/>
+      <c r="B10" s="1">
         <v>8</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="1">
         <v>10</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="3">
-        <v>1</v>
-      </c>
-      <c r="F10" s="3">
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="1"/>
-      <c r="B11" s="3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="1">
         <v>9</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="1">
         <v>11</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="1">
         <v>0</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="1"/>
-      <c r="B12" s="3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="1">
         <v>10</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="1">
         <v>12</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="3">
-        <v>1</v>
-      </c>
-      <c r="C18" s="3">
-        <v>9</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="3">
-        <v>1</v>
-      </c>
-      <c r="F18" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="1"/>
-      <c r="B19" s="3">
-        <v>2</v>
-      </c>
-      <c r="C19" s="3">
-        <v>9</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="3">
-        <v>1</v>
-      </c>
-      <c r="F19" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30">
-      <c r="A20" s="1"/>
-      <c r="B20" s="3">
-        <v>3</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0</v>
-      </c>
-      <c r="F20" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="1"/>
-      <c r="B21" s="3">
-        <v>4</v>
-      </c>
-      <c r="C21" s="3">
-        <v>11</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="3">
-        <v>0</v>
-      </c>
-      <c r="F21" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="1"/>
-      <c r="B22" s="3">
-        <v>5</v>
-      </c>
-      <c r="C22" s="3">
-        <v>12</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E22" s="3">
-        <v>1</v>
-      </c>
-      <c r="F22" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="1"/>
-      <c r="B23" s="3">
-        <v>6</v>
-      </c>
-      <c r="C23" s="3">
-        <v>23</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23" s="3">
-        <v>1</v>
-      </c>
-      <c r="F23" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="1"/>
-      <c r="B24" s="3">
-        <v>7</v>
-      </c>
-      <c r="C24" s="3">
-        <v>25</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="3">
-        <v>1</v>
-      </c>
-      <c r="F24" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="1"/>
-      <c r="B25" s="3">
-        <v>8</v>
-      </c>
-      <c r="C25" s="3">
-        <v>10</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="3">
-        <v>1</v>
-      </c>
-      <c r="F25" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="1"/>
-      <c r="B26" s="3">
-        <v>9</v>
-      </c>
-      <c r="C26" s="3">
-        <v>11</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="3">
-        <v>0</v>
-      </c>
-      <c r="F26" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="1"/>
-      <c r="B27" s="3">
-        <v>10</v>
-      </c>
-      <c r="C27" s="3">
-        <v>12</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="3">
-        <v>0</v>
-      </c>
-      <c r="F27" s="3">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A18:A27"/>
+  <mergeCells count="5">
     <mergeCell ref="A3:A12"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="A1:B2"/>
-    <mergeCell ref="A16:B17"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
bullbe add 20 to 40
</commit_message>
<xml_diff>
--- a/bubble_fault_seeded.xlsx
+++ b/bubble_fault_seeded.xlsx
@@ -289,8 +289,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -345,7 +351,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="41">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -363,6 +369,9 @@
     <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -380,6 +389,9 @@
     <cellStyle name="访问过的超链接" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -709,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -934,14 +946,68 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="E13">
+      <c r="B13" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="B16" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="1"/>
+      <c r="E23">
         <f>SUM(E3:E12)/COUNT(E3:E12)</f>
         <v>0.6</v>
       </c>
-      <c r="F13">
+      <c r="F23">
         <f>SUM(F3:F12)/COUNT(F3:F12)</f>
         <v>0.9</v>
       </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
dd 20 more faults in bubble test
</commit_message>
<xml_diff>
--- a/bubble_fault_seeded.xlsx
+++ b/bubble_fault_seeded.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <r>
       <t>if (array[d] &gt; array</t>
@@ -207,6 +207,141 @@
   </si>
   <si>
     <t>10-11</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>arr[pos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>] = temp;</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   for (c = 0; c &lt; ( n - 1 ); </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>c+=2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) {</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">for (c = 0; c </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ( n - 1 ); c++) {</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  for (d = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; d &lt; n - c - 1; d++) {</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   if (array[d] &gt; array[d-1])</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>swap(array, d-1, d+1);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    swap(array, d, d+1);break;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   for (c = -1; c &lt; ( n - 1 ); c++) {</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> add return array;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   n = array.length/2;</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -332,7 +467,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -350,6 +485,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="41">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
@@ -724,7 +861,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -946,68 +1083,201 @@
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="A13" s="1"/>
       <c r="B13" s="1">
         <v>11</v>
       </c>
+      <c r="C13" s="8">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="8">
+        <v>1</v>
+      </c>
+      <c r="F13" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="A14" s="1"/>
       <c r="B14" s="1">
         <v>12</v>
       </c>
+      <c r="C14" s="8">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0</v>
+      </c>
+      <c r="F14" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="A15" s="1"/>
       <c r="B15" s="1">
         <v>13</v>
       </c>
+      <c r="C15" s="8">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="8">
+        <v>1</v>
+      </c>
+      <c r="F15" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="A16" s="1"/>
       <c r="B16" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="2:6">
+      <c r="C16" s="8">
+        <v>11</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="8">
+        <v>1</v>
+      </c>
+      <c r="F16" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1"/>
       <c r="B17" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="2:6">
+      <c r="C17" s="8">
+        <v>12</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="8">
+        <v>1</v>
+      </c>
+      <c r="F17" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1"/>
       <c r="B18" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="2:6">
+      <c r="C18" s="8">
+        <v>14</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="8">
+        <v>1</v>
+      </c>
+      <c r="F18" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1"/>
       <c r="B19" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="2:6">
+      <c r="C19" s="8">
+        <v>14</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="8">
+        <v>1</v>
+      </c>
+      <c r="F19" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="2:6">
+      <c r="C20" s="8">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="8">
+        <v>1</v>
+      </c>
+      <c r="F20" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1"/>
       <c r="B21" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="2:6">
+      <c r="C21" s="8">
+        <v>17</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="8">
+        <v>1</v>
+      </c>
+      <c r="F21" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1"/>
       <c r="B22" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="2:6">
+      <c r="C22" s="8">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="8">
+        <v>1</v>
+      </c>
+      <c r="F22" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="E23">
-        <f>SUM(E3:E12)/COUNT(E3:E12)</f>
-        <v>0.6</v>
-      </c>
-      <c r="F23">
-        <f>SUM(F3:F12)/COUNT(F3:F12)</f>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1">
+        <f>SUM(E3:E22)/COUNT(E3:E22)</f>
+        <v>0.75</v>
+      </c>
+      <c r="F23" s="1">
+        <f>SUM(F3:F22)/COUNT(F3:F22)</f>
         <v>0.9</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
-      <c r="B24" s="1"/>
+    <row r="24" spans="1:6">
+      <c r="B24" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>